<commit_message>
updated_doing Search and Sort
</commit_message>
<xml_diff>
--- a/000_DSA_500.xlsx
+++ b/000_DSA_500.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\DSA_cracker 500\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Immediate\DSA_cracker 500\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADEB7BD-F61E-4FCD-914F-6A63CB2A3A28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D4DC3-3DD1-4931-A2E5-2CA2F6EFA753}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="531">
   <si>
     <t>Topic:</t>
   </si>
@@ -1588,6 +1588,36 @@
   </si>
   <si>
     <t xml:space="preserve">leetcode link </t>
+  </si>
+  <si>
+    <t>mark current cell as done</t>
+  </si>
+  <si>
+    <t>coding ninja 4511</t>
+  </si>
+  <si>
+    <t>added comment in code</t>
+  </si>
+  <si>
+    <t>min heap topic</t>
+  </si>
+  <si>
+    <t>use binary search to find the element, then traverse right and left using while loop for finding indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If not sorted use linear search, else use divide and conquer like binary search on mid indices if the value is same return else check which side you'll go, left or right </t>
+  </si>
+  <si>
+    <t>just square the I in for loop… it will logN operation</t>
+  </si>
+  <si>
+    <t>in notebook IMPORTANT QUES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See ques 2 in arrays… </t>
+  </si>
+  <si>
+    <t>copy and code</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1780,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1772,6 +1802,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1789,7 +1825,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1878,6 +1914,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2101,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3728,7 +3770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="18">
         <v>88</v>
       </c>
@@ -3742,7 +3784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="18">
         <v>89</v>
       </c>
@@ -3756,16 +3798,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="18"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="18"/>
       <c r="B100" s="6"/>
       <c r="C100" s="3"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="18">
         <v>90</v>
       </c>
@@ -3775,11 +3817,14 @@
       <c r="C101" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D101" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="20" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="18">
         <v>91</v>
       </c>
@@ -3789,11 +3834,14 @@
       <c r="C102" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D102" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="18">
         <v>92</v>
       </c>
@@ -3803,11 +3851,14 @@
       <c r="C103" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D103" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="18">
         <v>93</v>
       </c>
@@ -3817,25 +3868,31 @@
       <c r="C104" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D104" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="18">
         <v>94</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D105" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" s="20" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="18">
         <v>95</v>
       </c>
@@ -3849,7 +3906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="18">
         <v>96</v>
       </c>
@@ -3859,11 +3916,14 @@
       <c r="C107" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D107" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D107" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="20" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="18">
         <v>97</v>
       </c>
@@ -3877,7 +3937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="18">
         <v>98</v>
       </c>
@@ -3891,7 +3951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="18">
         <v>99</v>
       </c>
@@ -3905,7 +3965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="18">
         <v>100</v>
       </c>
@@ -3919,7 +3979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="18">
         <v>101</v>
       </c>
@@ -4287,7 +4347,7 @@
       <c r="C139" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4301,7 +4361,7 @@
       <c r="C140" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D140" s="4" t="s">
+      <c r="D140" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4315,7 +4375,7 @@
       <c r="C141" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D141" s="4" t="s">
+      <c r="D141" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4329,7 +4389,7 @@
       <c r="C142" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D142" s="4" t="s">
+      <c r="D142" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4343,7 +4403,7 @@
       <c r="C143" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="D143" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4357,7 +4417,7 @@
       <c r="C144" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D144" s="4" t="s">
+      <c r="D144" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4368,10 +4428,10 @@
       <c r="B145" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="C145" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="D145" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4385,7 +4445,7 @@
       <c r="C146" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="D146" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4399,7 +4459,7 @@
       <c r="C147" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D147" s="4" t="s">
+      <c r="D147" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4410,10 +4470,10 @@
       <c r="B148" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C148" s="5" t="s">
+      <c r="C148" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="D148" s="4" t="s">
+      <c r="D148" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4427,7 +4487,7 @@
       <c r="C149" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D149" s="4" t="s">
+      <c r="D149" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4441,7 +4501,7 @@
       <c r="C150" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D150" s="4" t="s">
+      <c r="D150" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4452,10 +4512,10 @@
       <c r="B151" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C151" s="5" t="s">
+      <c r="C151" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D151" s="4" t="s">
+      <c r="D151" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4469,7 +4529,7 @@
       <c r="C152" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D152" s="4" t="s">
+      <c r="D152" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4483,7 +4543,7 @@
       <c r="C153" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D153" s="4" t="s">
+      <c r="D153" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4494,10 +4554,10 @@
       <c r="B154" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C154" s="5" t="s">
+      <c r="C154" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="D154" s="4" t="s">
+      <c r="D154" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4508,10 +4568,10 @@
       <c r="B155" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C155" s="5" t="s">
+      <c r="C155" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="D155" s="4" t="s">
+      <c r="D155" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4522,10 +4582,10 @@
       <c r="B156" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C156" s="5" t="s">
+      <c r="C156" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="D156" s="4" t="s">
+      <c r="D156" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4539,7 +4599,7 @@
       <c r="C157" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D157" s="4" t="s">
+      <c r="D157" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4553,7 +4613,7 @@
       <c r="C158" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D158" s="4" t="s">
+      <c r="D158" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4567,7 +4627,7 @@
       <c r="C159" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D159" s="4" t="s">
+      <c r="D159" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4581,7 +4641,7 @@
       <c r="C160" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D160" s="4" t="s">
+      <c r="D160" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4595,8 +4655,8 @@
       <c r="C161" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D161" s="4" t="s">
-        <v>4</v>
+      <c r="D161" s="35" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -4606,10 +4666,10 @@
       <c r="B162" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C162" s="5" t="s">
+      <c r="C162" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D162" s="4" t="s">
+      <c r="D162" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4623,7 +4683,7 @@
       <c r="C163" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D163" s="4" t="s">
+      <c r="D163" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4637,7 +4697,7 @@
       <c r="C164" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D164" s="4" t="s">
+      <c r="D164" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4651,7 +4711,7 @@
       <c r="C165" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D165" s="4" t="s">
+      <c r="D165" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4665,7 +4725,7 @@
       <c r="C166" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D166" s="4" t="s">
+      <c r="D166" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4676,10 +4736,10 @@
       <c r="B167" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C167" s="5" t="s">
+      <c r="C167" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D167" s="4" t="s">
+      <c r="D167" s="34" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6099,17 +6159,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A273" s="18"/>
       <c r="C273" s="3"/>
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A274" s="18"/>
       <c r="C274" s="3"/>
       <c r="D274" s="4"/>
     </row>
-    <row r="275" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A275" s="18">
         <v>254</v>
       </c>
@@ -6119,11 +6179,17 @@
       <c r="C275" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D275" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D275" s="26">
+        <v>44273</v>
+      </c>
+      <c r="E275" s="20" t="s">
+        <v>521</v>
+      </c>
+      <c r="F275" s="20" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A276" s="18">
         <v>255</v>
       </c>
@@ -6133,11 +6199,17 @@
       <c r="C276" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D276" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D276" s="26">
+        <v>44273</v>
+      </c>
+      <c r="E276" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="F276" s="20" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A277" s="18">
         <v>256</v>
       </c>
@@ -6147,11 +6219,17 @@
       <c r="C277" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D277" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D277" s="26">
+        <v>44273</v>
+      </c>
+      <c r="E277" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="F277" s="20" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A278" s="18">
         <v>257</v>
       </c>
@@ -6165,7 +6243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A279" s="18">
         <v>258</v>
       </c>
@@ -6175,11 +6253,17 @@
       <c r="C279" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="D279" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="280" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D279" s="26">
+        <v>44273</v>
+      </c>
+      <c r="E279" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="F279" s="20" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A280" s="18">
         <v>259</v>
       </c>
@@ -6193,7 +6277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A281" s="18">
         <v>260</v>
       </c>
@@ -6207,7 +6291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A282" s="18">
         <v>261</v>
       </c>
@@ -6221,7 +6305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A283" s="18">
         <v>262</v>
       </c>
@@ -6235,7 +6319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A284" s="18">
         <v>263</v>
       </c>
@@ -6249,7 +6333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A285" s="18">
         <v>264</v>
       </c>
@@ -6263,7 +6347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A286" s="18">
         <v>265</v>
       </c>
@@ -6277,7 +6361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A287" s="18">
         <v>266</v>
       </c>
@@ -6291,7 +6375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A288" s="18">
         <v>267</v>
       </c>
@@ -9553,332 +9637,332 @@
     <hyperlink ref="C144" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
     <hyperlink ref="C145" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
     <hyperlink ref="C146" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="C147" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="C148" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="C149" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="C150" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="C151" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="C152" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="C153" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="C154" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="C155" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="C156" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="C157" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="C158" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="C159" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="C160" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="C161" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="C162" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="C163" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="C166" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="C167" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="C168" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="C169" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="C170" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="C171" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="C172" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="C173" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="C174" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="C177" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="C178" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="C179" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="C180" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="C181" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="C182" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="C183" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="C184" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="C185" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="C186" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="C187" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="C188" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="C189" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="C190" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="C191" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="C192" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="C193" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="C194" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="C195" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="C196" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="C197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="C198" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="C199" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="C200" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="C201" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="C202" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="C203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="C204" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="C205" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="C206" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="C207" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="C208" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="C209" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="C210" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="C211" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="C214" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="C215" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="C216" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="C217" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="C218" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="C219" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="C220" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="C221" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="C222" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="C223" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="C224" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="C225" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="C226" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="C227" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="C228" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="C229" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="C230" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="C231" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="C232" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="C233" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="C234" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="C235" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="C238" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="C239" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="C240" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="C241" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="C242" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="C243" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="C244" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="C245" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="C246" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="C247" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="C248" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="C249" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="C250" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="C251" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="C252" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="C253" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="C254" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="C255" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="C256" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="C257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="C258" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="C259" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="C260" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="C261" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="C262" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="C263" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="C264" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="C265" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="C266" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="C267" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="C268" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="C269" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="C270" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="C271" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="C272" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="C275" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="C276" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="C277" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="C278" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="C279" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="C280" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="C281" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="C282" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="C283" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="C284" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="C285" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="C286" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="C287" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="C288" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="C289" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="C290" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="C291" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="C292" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="C293" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="C296" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="C297" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="C298" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="C299" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="C300" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="C301" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="C302" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="C303" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="C304" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="C305" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="C306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="C307" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="C308" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="C309" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="C310" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="C311" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="C312" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="C313" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="C314" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="C315" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="C316" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="C317" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="C318" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="C319" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="C320" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="C321" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="C322" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="C323" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="C324" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="C325" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="C326" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="C327" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="C328" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="C329" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="C330" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="C331" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="C332" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="C333" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="C336" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="C337" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="C338" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="C339" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="C340" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="C341" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="C342" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="C343" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="C344" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="C345" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="C346" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="C347" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="C348" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="C349" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="C350" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="C351" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="C352" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="C353" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="C356" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="C357" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="C358" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="C359" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="C360" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="C361" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="C362" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="C363" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="C364" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="C365" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="C366" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="C367" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="C368" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="C369" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="C370" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="C371" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="C372" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="C373" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="C374" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="C375" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="C376" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="C377" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="C378" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="C379" r:id="rId349" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="C380" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="C381" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="C382" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="C383" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="C384" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="C385" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="C386" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="C387" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="C388" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="C389" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="C390" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="C391" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="C392" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="C393" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="C394" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="C395" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="C396" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="C397" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="C398" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="C399" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="C402" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="C403" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="C404" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="C405" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="C406" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="C407" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="C410" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="C411" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="C412" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="C413" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="C414" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="C415" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="C416" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="C417" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="C418" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="C419" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="C420" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="C421" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="C422" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="C423" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="C424" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="C425" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="C426" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="C427" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="C428" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="C429" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="C430" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="C431" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="C432" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="C433" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="C434" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="C435" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="C436" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="C437" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="C438" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="C439" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="C440" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="C441" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="C442" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="C443" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="C444" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="C445" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="C446" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="C447" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="C448" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="C449" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="C450" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="C451" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="C452" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="C453" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="C454" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="C455" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="C456" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="C457" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="C458" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="C459" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="C460" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="C461" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="C462" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="C463" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="C464" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="C465" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="C466" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="C467" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="C468" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="C469" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="C472" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="C473" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="C474" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="C475" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="C476" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="C477" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="C478" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="C479" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="C480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="C481" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="F17" r:id="rId446" xr:uid="{C2E4287D-6D0A-4CAD-870C-B3BEC3470BD9}"/>
-    <hyperlink ref="F35" r:id="rId447" xr:uid="{0526C445-85B2-43EE-927C-8E2A81BE67E6}"/>
-    <hyperlink ref="E35" r:id="rId448" display="set 1 article" xr:uid="{11425440-26AB-4CBC-8BE8-9F65717EC925}"/>
-    <hyperlink ref="E36" r:id="rId449" display="read this arcticle " xr:uid="{2E897128-5632-4045-8E5B-09FF43ABA268}"/>
-    <hyperlink ref="E37" r:id="rId450" xr:uid="{585BCAD9-624C-4E4C-8B2E-85CC93D5C85C}"/>
-    <hyperlink ref="E38" r:id="rId451" xr:uid="{0B7F77DD-BCAE-4285-9306-046E33CA76F0}"/>
-    <hyperlink ref="E39" r:id="rId452" xr:uid="{098DEF08-8658-40AF-9B02-65804B2DB8DE}"/>
-    <hyperlink ref="E40" r:id="rId453" xr:uid="{1654F358-DE23-4651-AD55-63A368DE090D}"/>
-    <hyperlink ref="E48" r:id="rId454" xr:uid="{228086FD-2CAB-4B2C-A5C9-498A90756123}"/>
-    <hyperlink ref="E52" r:id="rId455" display="YT video | binary seach and count " xr:uid="{AD10FD76-BA31-4FC1-B93B-FCA4DC2FF0EB}"/>
-    <hyperlink ref="F53" r:id="rId456" xr:uid="{C4B33961-31F9-4AE7-9B8B-3E05FD537ECC}"/>
-    <hyperlink ref="F63" r:id="rId457" xr:uid="{D5E84F02-8C03-4B34-9811-41B4BB9381D9}"/>
-    <hyperlink ref="F67" r:id="rId458" xr:uid="{311E5E6E-F3A2-48B0-BD41-F18671887BD2}"/>
+    <hyperlink ref="C148" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="C149" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="C150" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="C151" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="C152" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="C153" r:id="rId138" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="C154" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="C155" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="C156" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="C157" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="C158" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="C159" r:id="rId144" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="C160" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="C161" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="C162" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="C163" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="C166" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="C167" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="C168" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="C169" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="C170" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="C171" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="C172" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="C173" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="C174" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="C177" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="C178" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="C179" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="C180" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="C181" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="C182" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="C183" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="C184" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="C185" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="C186" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="C187" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="C188" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C189" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="C190" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="C191" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="C192" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="C193" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="C194" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="C195" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="C196" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="C197" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="C198" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="C199" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="C200" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="C201" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="C202" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="C203" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="C204" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="C205" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="C206" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="C207" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="C208" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="C209" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="C210" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="C211" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="C214" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="C215" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="C216" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="C217" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="C218" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="C219" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="C220" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="C221" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="C222" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="C223" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="C224" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="C225" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="C226" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="C227" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="C228" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="C229" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="C230" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="C231" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="C232" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="C233" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="C234" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="C235" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="C238" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="C239" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="C240" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="C241" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="C242" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="C243" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="C244" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="C245" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="C246" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="C247" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="C248" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="C249" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="C250" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="C251" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="C252" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="C253" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="C254" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="C255" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="C256" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="C257" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="C258" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="C259" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="C260" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="C261" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="C262" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C263" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="C264" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="C265" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C266" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="C267" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="C268" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="C269" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="C270" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="C271" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="C272" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="C275" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C276" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="C277" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="C278" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="C279" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="C280" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="C281" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="C282" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="C283" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="C284" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="C285" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="C286" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="C287" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="C288" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="C289" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="C290" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="C291" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="C292" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="C293" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="C296" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="C297" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="C298" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="C299" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="C300" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="C301" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="C302" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="C303" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="C304" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="C305" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="C306" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="C307" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="C308" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="C309" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="C310" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="C311" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="C312" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="C313" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="C314" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="C315" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="C316" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="C317" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="C318" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="C319" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="C320" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="C321" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="C322" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="C323" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="C324" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="C325" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="C326" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="C327" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="C328" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="C329" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="C330" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="C331" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="C332" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="C333" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="C336" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="C337" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="C338" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="C339" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="C340" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="C341" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="C342" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="C343" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="C344" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="C345" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="C346" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="C347" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="C348" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="C349" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="C350" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="C351" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="C352" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="C353" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="C356" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="C357" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="C358" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="C359" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="C360" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="C361" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="C362" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="C363" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="C364" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="C365" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="C366" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="C367" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="C368" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="C369" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="C370" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="C371" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="C372" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="C373" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="C374" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="C375" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="C376" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="C377" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="C378" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="C379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="C380" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="C381" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="C382" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="C383" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="C384" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="C385" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="C386" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="C387" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="C388" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="C389" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="C390" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="C391" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="C392" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="C393" r:id="rId362" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
+    <hyperlink ref="C394" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
+    <hyperlink ref="C395" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
+    <hyperlink ref="C396" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
+    <hyperlink ref="C397" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
+    <hyperlink ref="C398" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
+    <hyperlink ref="C399" r:id="rId368" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
+    <hyperlink ref="C402" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
+    <hyperlink ref="C403" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
+    <hyperlink ref="C404" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
+    <hyperlink ref="C405" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
+    <hyperlink ref="C406" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
+    <hyperlink ref="C407" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
+    <hyperlink ref="C410" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
+    <hyperlink ref="C411" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
+    <hyperlink ref="C412" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
+    <hyperlink ref="C413" r:id="rId378" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
+    <hyperlink ref="C414" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
+    <hyperlink ref="C415" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
+    <hyperlink ref="C416" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
+    <hyperlink ref="C417" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
+    <hyperlink ref="C418" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
+    <hyperlink ref="C419" r:id="rId384" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
+    <hyperlink ref="C420" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
+    <hyperlink ref="C421" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
+    <hyperlink ref="C422" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
+    <hyperlink ref="C423" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
+    <hyperlink ref="C424" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
+    <hyperlink ref="C425" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
+    <hyperlink ref="C426" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
+    <hyperlink ref="C427" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
+    <hyperlink ref="C428" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
+    <hyperlink ref="C429" r:id="rId394" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
+    <hyperlink ref="C430" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
+    <hyperlink ref="C431" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
+    <hyperlink ref="C432" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
+    <hyperlink ref="C433" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
+    <hyperlink ref="C434" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
+    <hyperlink ref="C435" r:id="rId400" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
+    <hyperlink ref="C436" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
+    <hyperlink ref="C437" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
+    <hyperlink ref="C438" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
+    <hyperlink ref="C439" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
+    <hyperlink ref="C440" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
+    <hyperlink ref="C441" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
+    <hyperlink ref="C442" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
+    <hyperlink ref="C443" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
+    <hyperlink ref="C444" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
+    <hyperlink ref="C445" r:id="rId410" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
+    <hyperlink ref="C446" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
+    <hyperlink ref="C447" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
+    <hyperlink ref="C448" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
+    <hyperlink ref="C449" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
+    <hyperlink ref="C450" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
+    <hyperlink ref="C451" r:id="rId416" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
+    <hyperlink ref="C452" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
+    <hyperlink ref="C453" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
+    <hyperlink ref="C454" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
+    <hyperlink ref="C455" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
+    <hyperlink ref="C456" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
+    <hyperlink ref="C457" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
+    <hyperlink ref="C458" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
+    <hyperlink ref="C459" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
+    <hyperlink ref="C460" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
+    <hyperlink ref="C461" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
+    <hyperlink ref="C462" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
+    <hyperlink ref="C463" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
+    <hyperlink ref="C464" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
+    <hyperlink ref="C465" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
+    <hyperlink ref="C466" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
+    <hyperlink ref="C467" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
+    <hyperlink ref="C468" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
+    <hyperlink ref="C469" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
+    <hyperlink ref="C472" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
+    <hyperlink ref="C473" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
+    <hyperlink ref="C474" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
+    <hyperlink ref="C475" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
+    <hyperlink ref="C476" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
+    <hyperlink ref="C477" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
+    <hyperlink ref="C478" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
+    <hyperlink ref="C479" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
+    <hyperlink ref="C480" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
+    <hyperlink ref="C481" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
+    <hyperlink ref="F17" r:id="rId445" xr:uid="{C2E4287D-6D0A-4CAD-870C-B3BEC3470BD9}"/>
+    <hyperlink ref="F35" r:id="rId446" xr:uid="{0526C445-85B2-43EE-927C-8E2A81BE67E6}"/>
+    <hyperlink ref="E35" r:id="rId447" display="set 1 article" xr:uid="{11425440-26AB-4CBC-8BE8-9F65717EC925}"/>
+    <hyperlink ref="E36" r:id="rId448" display="read this arcticle " xr:uid="{2E897128-5632-4045-8E5B-09FF43ABA268}"/>
+    <hyperlink ref="E37" r:id="rId449" xr:uid="{585BCAD9-624C-4E4C-8B2E-85CC93D5C85C}"/>
+    <hyperlink ref="E38" r:id="rId450" xr:uid="{0B7F77DD-BCAE-4285-9306-046E33CA76F0}"/>
+    <hyperlink ref="E39" r:id="rId451" xr:uid="{098DEF08-8658-40AF-9B02-65804B2DB8DE}"/>
+    <hyperlink ref="E40" r:id="rId452" xr:uid="{1654F358-DE23-4651-AD55-63A368DE090D}"/>
+    <hyperlink ref="E48" r:id="rId453" xr:uid="{228086FD-2CAB-4B2C-A5C9-498A90756123}"/>
+    <hyperlink ref="E52" r:id="rId454" display="YT video | binary seach and count " xr:uid="{AD10FD76-BA31-4FC1-B93B-FCA4DC2FF0EB}"/>
+    <hyperlink ref="F53" r:id="rId455" xr:uid="{C4B33961-31F9-4AE7-9B8B-3E05FD537ECC}"/>
+    <hyperlink ref="F63" r:id="rId456" xr:uid="{D5E84F02-8C03-4B34-9811-41B4BB9381D9}"/>
+    <hyperlink ref="F67" r:id="rId457" xr:uid="{311E5E6E-F3A2-48B0-BD41-F18671887BD2}"/>
+    <hyperlink ref="C147" r:id="rId458" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId459"/>

</xml_diff>